<commit_message>
23/06/2021 - Working model
Next: visualizations
</commit_message>
<xml_diff>
--- a/data_demand_forecast/glossary.xlsx
+++ b/data_demand_forecast/glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd297915e9a08dcf/Master of Energy Research/Github/ArchEnSys/data_demand_forecast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{4FFABF72-4D76-430A-A877-D8B3C3CB79E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31ADFE91-1659-49F2-A4D2-FE6812AB56FF}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{4FFABF72-4D76-430A-A877-D8B3C3CB79E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FDD931E-6D10-4AB7-8200-393BE2C2D255}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="3915" windowWidth="17100" windowHeight="10125" activeTab="2" xr2:uid="{10B4C132-BA54-4AEF-901E-13450E2530A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{10B4C132-BA54-4AEF-901E-13450E2530A5}"/>
   </bookViews>
   <sheets>
     <sheet name="region" sheetId="2" r:id="rId1"/>
@@ -140,19 +140,10 @@
     <t>PAPUA</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>NATIONAL</t>
-  </si>
-  <si>
     <t>SUMATERA</t>
   </si>
   <si>
     <t>JAVA</t>
-  </si>
-  <si>
-    <t>NUSA TENGGARA</t>
   </si>
   <si>
     <t>KALIMANTAN</t>
@@ -229,18 +220,9 @@
     <t>GW</t>
   </si>
   <si>
-    <t>TWh</t>
-  </si>
-  <si>
     <t>kWh</t>
   </si>
   <si>
-    <t>electricity_demand_twh</t>
-  </si>
-  <si>
-    <t>net_electricity_production_twh</t>
-  </si>
-  <si>
     <t>total_capacity_gw</t>
   </si>
   <si>
@@ -251,6 +233,24 @@
   </si>
   <si>
     <t>kwh_dem_percap</t>
+  </si>
+  <si>
+    <t>BALI_NT</t>
+  </si>
+  <si>
+    <t>MALUKU_PAPUA</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>GWh</t>
+  </si>
+  <si>
+    <t>net_electricity_production_gwh</t>
+  </si>
+  <si>
+    <t>electricity_demand_gwh</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -683,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -699,7 +699,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1496,145 +1496,145 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
26/06/2021 10:50 pm - ANN resurrected
Next: report
</commit_message>
<xml_diff>
--- a/data_demand_forecast/glossary.xlsx
+++ b/data_demand_forecast/glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd297915e9a08dcf/Master of Energy Research/Github/ArchEnSys/data_demand_forecast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{4FFABF72-4D76-430A-A877-D8B3C3CB79E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FDD931E-6D10-4AB7-8200-393BE2C2D255}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{4FFABF72-4D76-430A-A877-D8B3C3CB79E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7E5099D-F95A-420D-AFB7-47BDB06707B5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{10B4C132-BA54-4AEF-901E-13450E2530A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10B4C132-BA54-4AEF-901E-13450E2530A5}"/>
   </bookViews>
   <sheets>
     <sheet name="region" sheetId="2" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>SUMATERA</t>
   </si>
   <si>
-    <t>JAVA</t>
-  </si>
-  <si>
     <t>KALIMANTAN</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>electricity_demand_gwh</t>
+  </si>
+  <si>
+    <t>JAWA</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DD2135-08C2-4419-9C8B-28D4D05ECD79}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6373A52A-539A-4388-8D97-6B1A4039BCBA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1507,134 +1507,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
-        <v>47</v>
-      </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>